<commit_message>
code voor analyse toegevoegd
</commit_message>
<xml_diff>
--- a/NetworkScheduling/Assignment 1/1A. Path-based/HET WERKTTTTTT/InputLetters.xlsx
+++ b/NetworkScheduling/Assignment 1/1A. Path-based/HET WERKTTTTTT/InputLetters.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\woute\AirlinePlanning\NetworkScheduling\Assignment 1\1A. Path-based\HET WERKTTTTTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9E635AE-2441-4FB4-A0FF-4C7BB6BFF160}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4059AF9D-49A1-4D5C-AE30-E08A6EFB072F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17364" yWindow="2820" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arcs" sheetId="1" r:id="rId1"/>
-    <sheet name="Commodities" sheetId="2" r:id="rId2"/>
+    <sheet name="Arcs2" sheetId="3" r:id="rId2"/>
+    <sheet name="Commodities" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arcs!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Commodities!$A$1:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Commodities!$A$1:$D$41</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="23">
   <si>
     <t>From</t>
   </si>
@@ -90,6 +91,15 @@
   </si>
   <si>
     <t>Quant</t>
+  </si>
+  <si>
+    <t>Arc</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Capacity</t>
   </si>
 </sst>
 </file>
@@ -456,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -900,6 +910,548 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3D6644-774F-4FD0-B592-D03A581B0EDC}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1">
+        <v>17</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="1">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="1">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1">
+        <v>13</v>
+      </c>
+      <c r="E18" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>22</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="1">
+        <v>12</v>
+      </c>
+      <c r="E22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="1">
+        <v>9</v>
+      </c>
+      <c r="E26" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="1">
+        <v>10</v>
+      </c>
+      <c r="E27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6</v>
+      </c>
+      <c r="E28" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="1">
+        <v>3</v>
+      </c>
+      <c r="E29" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="1">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>

</xml_diff>